<commit_message>
update mintapi package, add running net income
</commit_message>
<xml_diff>
--- a/Mint Categories Mapping.xlsx
+++ b/Mint Categories Mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="120" windowWidth="27320" windowHeight="12280"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="131">
   <si>
     <t>Discretionary</t>
   </si>
@@ -403,6 +403,18 @@
   </si>
   <si>
     <t>Other Taxes</t>
+  </si>
+  <si>
+    <t>Dividend &amp; Cap Gains</t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Sell</t>
   </si>
 </sst>
 </file>
@@ -459,8 +471,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="95">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -560,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="95">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -608,6 +624,8 @@
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -655,6 +673,8 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -954,11 +974,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B120" sqref="B120"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2317,7 +2337,51 @@
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>0</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>127</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>128</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>129</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>130</v>
+      </c>
+      <c r="B127" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>